<commit_message>
Fix a few issues for optimisation
</commit_message>
<xml_diff>
--- a/autumn/xls/data_default.xlsx
+++ b/autumn/xls/data_default.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20339"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20346"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rrag0004\Models\jtrauer_AuTuMN\autumn\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{944C4B32-88A9-4936-9612-8CAE232279DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C72120-433D-4124-B285-DC13189A5F9A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="915" windowWidth="20370" windowHeight="6930" tabRatio="807" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="920" windowWidth="20370" windowHeight="6930" tabRatio="807" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="4" r:id="rId1"/>
@@ -3235,18 +3235,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G280"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A100" sqref="A100"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="51.28515625" customWidth="1"/>
+    <col min="1" max="1" width="51.26953125" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="5" max="5" width="93.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="93.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="36" t="s">
         <v>9</v>
       </c>
@@ -3263,7 +3263,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="22" t="s">
         <v>11</v>
       </c>
@@ -3280,7 +3280,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="22" t="s">
         <v>13</v>
       </c>
@@ -3291,7 +3291,7 @@
       <c r="D3" s="23"/>
       <c r="E3" s="24"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="22" t="s">
         <v>56</v>
       </c>
@@ -3302,7 +3302,7 @@
       <c r="D4" s="23"/>
       <c r="E4" s="24"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="22" t="s">
         <v>57</v>
       </c>
@@ -3313,7 +3313,7 @@
       <c r="D5" s="23"/>
       <c r="E5" s="24"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="22" t="s">
         <v>268</v>
       </c>
@@ -3326,7 +3326,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="22" t="s">
         <v>14</v>
       </c>
@@ -3337,7 +3337,7 @@
       <c r="D7" s="23"/>
       <c r="E7" s="24"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="22" t="s">
         <v>52</v>
       </c>
@@ -3348,7 +3348,7 @@
       <c r="D8" s="23"/>
       <c r="E8" s="24"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="22" t="s">
         <v>53</v>
       </c>
@@ -3359,7 +3359,7 @@
       <c r="D9" s="23"/>
       <c r="E9" s="24"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="22" t="s">
         <v>54</v>
       </c>
@@ -3370,7 +3370,7 @@
       <c r="D10" s="23"/>
       <c r="E10" s="24"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="22" t="s">
         <v>15</v>
       </c>
@@ -3385,7 +3385,7 @@
       </c>
       <c r="E11" s="24"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="22" t="s">
         <v>136</v>
       </c>
@@ -3397,7 +3397,7 @@
       <c r="D12" s="23"/>
       <c r="E12" s="24"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="22" t="s">
         <v>16</v>
       </c>
@@ -3408,7 +3408,7 @@
       <c r="D13" s="23"/>
       <c r="E13" s="24"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="22" t="s">
         <v>17</v>
       </c>
@@ -3420,12 +3420,12 @@
       <c r="D14" s="23"/>
       <c r="E14" s="24"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="24" t="s">
         <v>322</v>
       </c>
       <c r="B15" s="25">
-        <v>0.6</v>
+        <v>0.99</v>
       </c>
       <c r="C15" s="25">
         <v>0.48</v>
@@ -3437,7 +3437,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="24" t="s">
         <v>137</v>
       </c>
@@ -3448,12 +3448,12 @@
       <c r="D16" s="25"/>
       <c r="E16" s="24"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="24" t="s">
         <v>321</v>
       </c>
       <c r="B17" s="25">
-        <v>0.75</v>
+        <v>0.99</v>
       </c>
       <c r="C17" s="25">
         <v>0.7</v>
@@ -3463,12 +3463,12 @@
       </c>
       <c r="E17" s="24"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="24" t="s">
         <v>319</v>
       </c>
       <c r="B18" s="25">
-        <v>0.76900000000000002</v>
+        <v>0.7</v>
       </c>
       <c r="C18" s="25">
         <v>0.56299999999999994</v>
@@ -3480,7 +3480,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="22" t="s">
         <v>142</v>
       </c>
@@ -3493,7 +3493,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="22" t="s">
         <v>290</v>
       </c>
@@ -3504,7 +3504,7 @@
       <c r="D20" s="23"/>
       <c r="E20" s="24"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="22" t="s">
         <v>138</v>
       </c>
@@ -3515,7 +3515,7 @@
       <c r="D21" s="23"/>
       <c r="E21" s="24"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="22" t="s">
         <v>307</v>
       </c>
@@ -3530,7 +3530,7 @@
       </c>
       <c r="E22" s="24"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="22" t="s">
         <v>19</v>
       </c>
@@ -3542,7 +3542,7 @@
       <c r="D23" s="23"/>
       <c r="E23" s="24"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="22" t="s">
         <v>20</v>
       </c>
@@ -3557,7 +3557,7 @@
       </c>
       <c r="E24" s="24"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="22" t="s">
         <v>144</v>
       </c>
@@ -3568,7 +3568,7 @@
       <c r="D25" s="23"/>
       <c r="E25" s="24"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="22" t="s">
         <v>145</v>
       </c>
@@ -3579,7 +3579,7 @@
       <c r="D26" s="23"/>
       <c r="E26" s="24"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="22" t="s">
         <v>146</v>
       </c>
@@ -3590,7 +3590,7 @@
       <c r="D27" s="23"/>
       <c r="E27" s="24"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="22" t="s">
         <v>21</v>
       </c>
@@ -3601,7 +3601,7 @@
       <c r="D28" s="23"/>
       <c r="E28" s="24"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="22" t="s">
         <v>22</v>
       </c>
@@ -3613,7 +3613,7 @@
       <c r="D29" s="23"/>
       <c r="E29" s="24"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="22" t="s">
         <v>23</v>
       </c>
@@ -3625,7 +3625,7 @@
       <c r="D30" s="23"/>
       <c r="E30" s="24"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="22" t="s">
         <v>313</v>
       </c>
@@ -3637,7 +3637,7 @@
       <c r="D31" s="23"/>
       <c r="E31" s="24"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="22" t="s">
         <v>24</v>
       </c>
@@ -3649,7 +3649,7 @@
       <c r="D32" s="23"/>
       <c r="E32" s="24"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="22" t="s">
         <v>62</v>
       </c>
@@ -3661,7 +3661,7 @@
       <c r="D33" s="23"/>
       <c r="E33" s="24"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="22" t="s">
         <v>61</v>
       </c>
@@ -3673,7 +3673,7 @@
       <c r="D34" s="23"/>
       <c r="E34" s="24"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="22" t="s">
         <v>55</v>
       </c>
@@ -3685,7 +3685,7 @@
       <c r="D35" s="23"/>
       <c r="E35" s="24"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="22" t="s">
         <v>184</v>
       </c>
@@ -3696,12 +3696,12 @@
       <c r="D36" s="23"/>
       <c r="E36" s="24"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="22" t="s">
         <v>320</v>
       </c>
       <c r="B37" s="23">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="C37" s="23">
         <v>0.4</v>
@@ -3711,7 +3711,7 @@
       </c>
       <c r="E37" s="24"/>
     </row>
-    <row r="38" spans="1:5" s="75" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" s="75" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A38" s="85" t="s">
         <v>329</v>
       </c>
@@ -3725,12 +3725,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:5" s="75" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" s="75" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A39" s="85" t="s">
         <v>330</v>
       </c>
       <c r="B39" s="23">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="C39" s="75">
         <v>0.35</v>
@@ -3739,7 +3739,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="40" spans="1:5" s="75" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" s="75" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A40" s="85" t="s">
         <v>331</v>
       </c>
@@ -3747,18 +3747,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="22" t="s">
         <v>279</v>
       </c>
       <c r="B41" s="23">
-        <v>0.95</v>
+        <v>0.99990000000000001</v>
       </c>
       <c r="C41" s="23"/>
       <c r="D41" s="23"/>
       <c r="E41" s="24"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="22" t="s">
         <v>303</v>
       </c>
@@ -3769,7 +3769,7 @@
       <c r="D42" s="23"/>
       <c r="E42" s="24"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="22" t="s">
         <v>314</v>
       </c>
@@ -3780,7 +3780,7 @@
       <c r="D43" s="23"/>
       <c r="E43" s="24"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="22" t="s">
         <v>315</v>
       </c>
@@ -3791,7 +3791,7 @@
       <c r="D44" s="23"/>
       <c r="E44" s="24"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="24" t="s">
         <v>254</v>
       </c>
@@ -3809,7 +3809,7 @@
       </c>
       <c r="E45" s="24"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="24" t="s">
         <v>255</v>
       </c>
@@ -3820,7 +3820,7 @@
       <c r="D46" s="25"/>
       <c r="E46" s="24"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="22" t="s">
         <v>8</v>
       </c>
@@ -3832,7 +3832,7 @@
       <c r="D47" s="23"/>
       <c r="E47" s="24"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="22" t="s">
         <v>6</v>
       </c>
@@ -3844,7 +3844,7 @@
       <c r="D48" s="23"/>
       <c r="E48" s="24"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="22" t="s">
         <v>7</v>
       </c>
@@ -3856,7 +3856,7 @@
       <c r="D49" s="23"/>
       <c r="E49" s="24"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="22" t="s">
         <v>26</v>
       </c>
@@ -3869,7 +3869,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="22" t="s">
         <v>28</v>
       </c>
@@ -3882,7 +3882,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="22" t="s">
         <v>139</v>
       </c>
@@ -3894,7 +3894,7 @@
       <c r="D52" s="23"/>
       <c r="E52" s="24"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="26" t="s">
         <v>30</v>
       </c>
@@ -3907,12 +3907,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="26" t="s">
         <v>256</v>
       </c>
       <c r="B54" s="27">
-        <v>0.43</v>
+        <v>0.99</v>
       </c>
       <c r="C54" s="27">
         <v>0.21</v>
@@ -3924,7 +3924,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="26" t="s">
         <v>327</v>
       </c>
@@ -3941,7 +3941,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="26" t="s">
         <v>326</v>
       </c>
@@ -3958,18 +3958,18 @@
         <v>309</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="26" t="s">
         <v>310</v>
       </c>
       <c r="B57" s="27">
-        <v>0.91</v>
+        <v>0.99</v>
       </c>
       <c r="C57" s="27"/>
       <c r="D57" s="27"/>
       <c r="E57" s="24"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="26" t="s">
         <v>257</v>
       </c>
@@ -3986,7 +3986,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="26" t="s">
         <v>258</v>
       </c>
@@ -3997,7 +3997,7 @@
       <c r="D59" s="27"/>
       <c r="E59" s="24"/>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="26" t="s">
         <v>259</v>
       </c>
@@ -4010,7 +4010,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="26" t="s">
         <v>260</v>
       </c>
@@ -4023,7 +4023,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="26" t="s">
         <v>325</v>
       </c>
@@ -4041,7 +4041,7 @@
       </c>
       <c r="E62" s="24"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="26" t="s">
         <v>324</v>
       </c>
@@ -4061,7 +4061,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="26" t="s">
         <v>261</v>
       </c>
@@ -4078,7 +4078,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="26" t="s">
         <v>312</v>
       </c>
@@ -4095,7 +4095,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="26" t="s">
         <v>361</v>
       </c>
@@ -4112,7 +4112,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="26" t="s">
         <v>328</v>
       </c>
@@ -4123,7 +4123,7 @@
       <c r="D67" s="27"/>
       <c r="E67" s="24"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="26" t="s">
         <v>228</v>
       </c>
@@ -4134,7 +4134,7 @@
       <c r="D68" s="27"/>
       <c r="E68" s="24"/>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="26" t="s">
         <v>227</v>
       </c>
@@ -4145,7 +4145,7 @@
       <c r="D69" s="27"/>
       <c r="E69" s="24"/>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="26" t="s">
         <v>226</v>
       </c>
@@ -4156,7 +4156,7 @@
       <c r="D70" s="27"/>
       <c r="E70" s="24"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="26" t="s">
         <v>225</v>
       </c>
@@ -4167,7 +4167,7 @@
       <c r="D71" s="27"/>
       <c r="E71" s="24"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="26" t="s">
         <v>229</v>
       </c>
@@ -4178,7 +4178,7 @@
       <c r="D72" s="27"/>
       <c r="E72" s="24"/>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="26" t="s">
         <v>230</v>
       </c>
@@ -4189,7 +4189,7 @@
       <c r="D73" s="27"/>
       <c r="E73" s="24"/>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="90" t="s">
         <v>363</v>
       </c>
@@ -4202,7 +4202,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="22" t="s">
         <v>335</v>
       </c>
@@ -4213,7 +4213,7 @@
       <c r="D75" s="75"/>
       <c r="E75" s="75"/>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="22" t="s">
         <v>336</v>
       </c>
@@ -4224,7 +4224,7 @@
       <c r="D76" s="75"/>
       <c r="E76" s="75"/>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" s="22" t="s">
         <v>334</v>
       </c>
@@ -4235,7 +4235,7 @@
       <c r="D77" s="75"/>
       <c r="E77" s="75"/>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" s="26" t="s">
         <v>262</v>
       </c>
@@ -4249,7 +4249,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" s="26" t="s">
         <v>263</v>
       </c>
@@ -4262,12 +4262,12 @@
         <v>133</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" s="26" t="s">
         <v>264</v>
       </c>
       <c r="B80" s="27">
-        <v>0.75</v>
+        <v>0.9</v>
       </c>
       <c r="C80" s="27">
         <v>0.65</v>
@@ -4279,7 +4279,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" s="26" t="s">
         <v>311</v>
       </c>
@@ -4294,18 +4294,18 @@
       </c>
       <c r="E81" s="24"/>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" s="26" t="s">
         <v>265</v>
       </c>
       <c r="B82" s="27">
-        <v>0.27</v>
+        <v>0.1</v>
       </c>
       <c r="C82" s="27"/>
       <c r="D82" s="27"/>
       <c r="E82" s="24"/>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" s="26" t="s">
         <v>266</v>
       </c>
@@ -4316,7 +4316,7 @@
       <c r="D83" s="27"/>
       <c r="E83" s="24"/>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" s="24" t="s">
         <v>177</v>
       </c>
@@ -4329,7 +4329,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" s="24" t="s">
         <v>359</v>
       </c>
@@ -4340,7 +4340,7 @@
       <c r="D85" s="25"/>
       <c r="E85" s="24"/>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" s="24" t="s">
         <v>360</v>
       </c>
@@ -4351,7 +4351,7 @@
       <c r="D86" s="25"/>
       <c r="E86" s="24"/>
     </row>
-    <row r="87" spans="1:5" s="67" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" s="67" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A87" s="24" t="s">
         <v>178</v>
       </c>
@@ -4362,7 +4362,7 @@
       <c r="D87" s="25"/>
       <c r="E87" s="24"/>
     </row>
-    <row r="88" spans="1:5" s="67" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" s="67" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A88" s="24" t="s">
         <v>179</v>
       </c>
@@ -4373,7 +4373,7 @@
       <c r="D88" s="25"/>
       <c r="E88" s="24"/>
     </row>
-    <row r="89" spans="1:5" s="67" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" s="67" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A89" s="24" t="s">
         <v>180</v>
       </c>
@@ -4384,7 +4384,7 @@
       <c r="D89" s="25"/>
       <c r="E89" s="24"/>
     </row>
-    <row r="90" spans="1:5" s="67" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" s="67" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A90" s="24" t="s">
         <v>181</v>
       </c>
@@ -4395,7 +4395,7 @@
       <c r="D90" s="25"/>
       <c r="E90" s="24"/>
     </row>
-    <row r="91" spans="1:5" s="67" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" s="67" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A91" s="24" t="s">
         <v>182</v>
       </c>
@@ -4406,7 +4406,7 @@
       <c r="D91" s="25"/>
       <c r="E91" s="24"/>
     </row>
-    <row r="92" spans="1:5" s="67" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" s="67" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A92" s="24" t="s">
         <v>183</v>
       </c>
@@ -4417,7 +4417,7 @@
       <c r="D92" s="25"/>
       <c r="E92" s="24"/>
     </row>
-    <row r="93" spans="1:5" s="67" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" s="67" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A93" s="24" t="s">
         <v>365</v>
       </c>
@@ -4428,7 +4428,7 @@
       <c r="D93" s="25"/>
       <c r="E93" s="24"/>
     </row>
-    <row r="94" spans="1:5" s="67" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" s="67" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A94" s="24" t="s">
         <v>270</v>
       </c>
@@ -4439,7 +4439,7 @@
       <c r="D94" s="25"/>
       <c r="E94" s="24"/>
     </row>
-    <row r="95" spans="1:5" s="67" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" s="67" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A95" s="24" t="s">
         <v>276</v>
       </c>
@@ -4450,7 +4450,7 @@
       <c r="D95" s="25"/>
       <c r="E95" s="24"/>
     </row>
-    <row r="96" spans="1:5" s="67" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" s="67" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A96" s="24" t="s">
         <v>271</v>
       </c>
@@ -4461,7 +4461,7 @@
       <c r="D96" s="25"/>
       <c r="E96" s="24"/>
     </row>
-    <row r="97" spans="1:5" s="67" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" s="67" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A97" s="24" t="s">
         <v>272</v>
       </c>
@@ -4472,7 +4472,7 @@
       <c r="D97" s="25"/>
       <c r="E97" s="24"/>
     </row>
-    <row r="98" spans="1:5" s="67" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" s="67" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A98" s="24" t="s">
         <v>277</v>
       </c>
@@ -4483,7 +4483,7 @@
       <c r="D98" s="25"/>
       <c r="E98" s="24"/>
     </row>
-    <row r="99" spans="1:5" s="67" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" s="67" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A99" s="24" t="s">
         <v>273</v>
       </c>
@@ -4494,7 +4494,7 @@
       <c r="D99" s="25"/>
       <c r="E99" s="24"/>
     </row>
-    <row r="100" spans="1:5" s="67" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" s="67" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A100" s="24" t="s">
         <v>274</v>
       </c>
@@ -4505,7 +4505,7 @@
       <c r="D100" s="25"/>
       <c r="E100" s="24"/>
     </row>
-    <row r="101" spans="1:5" s="67" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" s="67" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A101" s="24" t="s">
         <v>278</v>
       </c>
@@ -4516,7 +4516,7 @@
       <c r="D101" s="25"/>
       <c r="E101" s="24"/>
     </row>
-    <row r="102" spans="1:5" s="67" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" s="67" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A102" s="24" t="s">
         <v>275</v>
       </c>
@@ -4527,7 +4527,7 @@
       <c r="D102" s="25"/>
       <c r="E102" s="24"/>
     </row>
-    <row r="103" spans="1:5" s="67" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" s="67" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A103" s="28" t="s">
         <v>275</v>
       </c>
@@ -4538,7 +4538,7 @@
       <c r="D103" s="29"/>
       <c r="E103" s="28"/>
     </row>
-    <row r="104" spans="1:5" s="67" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" s="67" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A104" s="28" t="s">
         <v>377</v>
       </c>
@@ -4549,7 +4549,7 @@
       <c r="D104" s="25"/>
       <c r="E104" s="24"/>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105" s="28" t="s">
         <v>378</v>
       </c>
@@ -4557,7 +4557,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106" s="30" t="s">
         <v>32</v>
       </c>
@@ -4574,7 +4574,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107" s="30" t="s">
         <v>58</v>
       </c>
@@ -4587,7 +4587,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108" s="30" t="s">
         <v>40</v>
       </c>
@@ -4598,7 +4598,7 @@
       <c r="D108" s="57"/>
       <c r="E108" s="30"/>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A109" s="30" t="s">
         <v>316</v>
       </c>
@@ -4609,7 +4609,7 @@
       <c r="D109" s="57"/>
       <c r="E109" s="30"/>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110" s="30" t="s">
         <v>41</v>
       </c>
@@ -4620,7 +4620,7 @@
       <c r="D110" s="57"/>
       <c r="E110" s="30"/>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A111" s="30" t="s">
         <v>34</v>
       </c>
@@ -4633,7 +4633,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A112" s="30" t="s">
         <v>36</v>
       </c>
@@ -4646,7 +4646,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A113" s="30" t="s">
         <v>42</v>
       </c>
@@ -4657,7 +4657,7 @@
       <c r="D113" s="57"/>
       <c r="E113" s="30"/>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A114" s="32" t="s">
         <v>323</v>
       </c>
@@ -4670,7 +4670,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A115" s="32" t="s">
         <v>93</v>
       </c>
@@ -4683,7 +4683,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A116" s="30" t="s">
         <v>125</v>
       </c>
@@ -4696,7 +4696,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A117" s="30" t="s">
         <v>85</v>
       </c>
@@ -4709,7 +4709,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A118" s="30" t="s">
         <v>86</v>
       </c>
@@ -4722,7 +4722,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A119" s="30" t="s">
         <v>89</v>
       </c>
@@ -4735,7 +4735,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A120" s="30" t="s">
         <v>112</v>
       </c>
@@ -4748,7 +4748,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A121" s="30" t="s">
         <v>113</v>
       </c>
@@ -4761,7 +4761,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A122" s="30" t="s">
         <v>114</v>
       </c>
@@ -4774,7 +4774,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A123" s="30" t="s">
         <v>100</v>
       </c>
@@ -4787,7 +4787,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A124" s="30" t="s">
         <v>143</v>
       </c>
@@ -4798,7 +4798,7 @@
       <c r="D124" s="57"/>
       <c r="E124" s="30"/>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A125" s="30" t="s">
         <v>98</v>
       </c>
@@ -4811,7 +4811,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A126" s="30" t="s">
         <v>65</v>
       </c>
@@ -4824,7 +4824,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A127" s="34" t="s">
         <v>43</v>
       </c>
@@ -4837,7 +4837,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A128" s="38" t="s">
         <v>45</v>
       </c>
@@ -4850,7 +4850,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A129" s="38" t="s">
         <v>49</v>
       </c>
@@ -4859,7 +4859,7 @@
       <c r="D129" s="38"/>
       <c r="E129" s="38"/>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A130" s="53" t="s">
         <v>64</v>
       </c>
@@ -4872,7 +4872,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A131" s="55" t="s">
         <v>67</v>
       </c>
@@ -4885,7 +4885,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A132" s="55" t="s">
         <v>73</v>
       </c>
@@ -4898,7 +4898,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A133" s="55" t="s">
         <v>118</v>
       </c>
@@ -4909,7 +4909,7 @@
       <c r="D133" s="61"/>
       <c r="E133" s="55"/>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A134" s="55" t="s">
         <v>127</v>
       </c>
@@ -4922,7 +4922,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A135" s="55" t="s">
         <v>79</v>
       </c>
@@ -4933,7 +4933,7 @@
       <c r="D135" s="61"/>
       <c r="E135" s="55"/>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A136" s="55" t="s">
         <v>70</v>
       </c>
@@ -4946,7 +4946,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A137" s="55" t="s">
         <v>74</v>
       </c>
@@ -4957,7 +4957,7 @@
       <c r="D137" s="61"/>
       <c r="E137" s="55"/>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A138" s="55" t="s">
         <v>119</v>
       </c>
@@ -4970,7 +4970,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A139" s="55" t="s">
         <v>132</v>
       </c>
@@ -4981,7 +4981,7 @@
       <c r="D139" s="63"/>
       <c r="E139" s="52"/>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A140" s="55" t="s">
         <v>80</v>
       </c>
@@ -4994,7 +4994,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A141" s="56" t="s">
         <v>68</v>
       </c>
@@ -5005,7 +5005,7 @@
       <c r="D141" s="63"/>
       <c r="E141" s="52"/>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A142" s="56" t="s">
         <v>75</v>
       </c>
@@ -5016,7 +5016,7 @@
       <c r="D142" s="63"/>
       <c r="E142" s="52"/>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A143" s="56" t="s">
         <v>120</v>
       </c>
@@ -5027,7 +5027,7 @@
       <c r="D143" s="63"/>
       <c r="E143" s="52"/>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A144" s="55" t="s">
         <v>128</v>
       </c>
@@ -5038,7 +5038,7 @@
       <c r="D144" s="63"/>
       <c r="E144" s="52"/>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A145" s="56" t="s">
         <v>81</v>
       </c>
@@ -5049,7 +5049,7 @@
       <c r="D145" s="63"/>
       <c r="E145" s="52"/>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A146" s="56" t="s">
         <v>69</v>
       </c>
@@ -5060,7 +5060,7 @@
       <c r="D146" s="63"/>
       <c r="E146" s="52"/>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A147" s="56" t="s">
         <v>76</v>
       </c>
@@ -5071,7 +5071,7 @@
       <c r="D147" s="63"/>
       <c r="E147" s="52"/>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A148" s="56" t="s">
         <v>121</v>
       </c>
@@ -5082,7 +5082,7 @@
       <c r="D148" s="63"/>
       <c r="E148" s="52"/>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A149" s="55" t="s">
         <v>129</v>
       </c>
@@ -5093,7 +5093,7 @@
       <c r="D149" s="63"/>
       <c r="E149" s="52"/>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A150" s="56" t="s">
         <v>82</v>
       </c>
@@ -5104,7 +5104,7 @@
       <c r="D150" s="63"/>
       <c r="E150" s="52"/>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A151" s="56" t="s">
         <v>71</v>
       </c>
@@ -5115,7 +5115,7 @@
       <c r="D151" s="63"/>
       <c r="E151" s="52"/>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A152" s="56" t="s">
         <v>77</v>
       </c>
@@ -5126,7 +5126,7 @@
       <c r="D152" s="63"/>
       <c r="E152" s="65"/>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A153" s="56" t="s">
         <v>122</v>
       </c>
@@ -5137,7 +5137,7 @@
       <c r="D153" s="63"/>
       <c r="E153" s="65"/>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A154" s="55" t="s">
         <v>130</v>
       </c>
@@ -5148,7 +5148,7 @@
       <c r="D154" s="63"/>
       <c r="E154" s="52"/>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A155" s="56" t="s">
         <v>83</v>
       </c>
@@ -5159,7 +5159,7 @@
       <c r="D155" s="63"/>
       <c r="E155" s="52"/>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A156" s="56" t="s">
         <v>72</v>
       </c>
@@ -5170,7 +5170,7 @@
       <c r="D156" s="61"/>
       <c r="E156" s="55"/>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A157" s="56" t="s">
         <v>78</v>
       </c>
@@ -5181,7 +5181,7 @@
       <c r="D157" s="61"/>
       <c r="E157" s="55"/>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A158" s="56" t="s">
         <v>123</v>
       </c>
@@ -5192,7 +5192,7 @@
       <c r="D158" s="61"/>
       <c r="E158" s="55"/>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A159" s="55" t="s">
         <v>134</v>
       </c>
@@ -5203,7 +5203,7 @@
       <c r="D159" s="61"/>
       <c r="E159" s="55"/>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A160" s="56" t="s">
         <v>84</v>
       </c>
@@ -5214,7 +5214,7 @@
       <c r="D160" s="61"/>
       <c r="E160" s="55"/>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A161" s="56" t="s">
         <v>109</v>
       </c>
@@ -5225,7 +5225,7 @@
       <c r="D161" s="61"/>
       <c r="E161" s="55"/>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A162" s="56" t="s">
         <v>110</v>
       </c>
@@ -5236,7 +5236,7 @@
       <c r="D162" s="61"/>
       <c r="E162" s="55"/>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A163" s="56" t="s">
         <v>124</v>
       </c>
@@ -5247,7 +5247,7 @@
       <c r="D163" s="61"/>
       <c r="E163" s="55"/>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A164" s="55" t="s">
         <v>131</v>
       </c>
@@ -5258,7 +5258,7 @@
       <c r="D164" s="61"/>
       <c r="E164" s="55"/>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A165" s="56" t="s">
         <v>111</v>
       </c>
@@ -5269,7 +5269,7 @@
       <c r="D165" s="61"/>
       <c r="E165" s="55"/>
     </row>
-    <row r="166" spans="1:7" s="68" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:7" s="68" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A166" s="55" t="s">
         <v>151</v>
       </c>
@@ -5280,7 +5280,7 @@
       <c r="D166" s="72"/>
       <c r="E166" s="70"/>
     </row>
-    <row r="167" spans="1:7" s="68" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:7" s="68" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A167" s="55" t="s">
         <v>150</v>
       </c>
@@ -5291,7 +5291,7 @@
       <c r="D167" s="72"/>
       <c r="E167" s="70"/>
     </row>
-    <row r="168" spans="1:7" s="68" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:7" s="68" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A168" s="55" t="s">
         <v>149</v>
       </c>
@@ -5302,7 +5302,7 @@
       <c r="D168" s="72"/>
       <c r="E168" s="70"/>
     </row>
-    <row r="169" spans="1:7" s="68" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:7" s="68" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A169" s="55" t="s">
         <v>148</v>
       </c>
@@ -5313,7 +5313,7 @@
       <c r="D169" s="72"/>
       <c r="E169" s="70"/>
     </row>
-    <row r="170" spans="1:7" s="68" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:7" s="68" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A170" s="55" t="s">
         <v>147</v>
       </c>
@@ -5324,7 +5324,7 @@
       <c r="D170" s="72"/>
       <c r="E170" s="70"/>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A171" s="55" t="s">
         <v>156</v>
       </c>
@@ -5337,7 +5337,7 @@
       <c r="F171" s="67"/>
       <c r="G171" s="67"/>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A172" s="55" t="s">
         <v>155</v>
       </c>
@@ -5350,7 +5350,7 @@
       <c r="F172" s="67"/>
       <c r="G172" s="67"/>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A173" s="55" t="s">
         <v>154</v>
       </c>
@@ -5363,7 +5363,7 @@
       <c r="F173" s="67"/>
       <c r="G173" s="67"/>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A174" s="55" t="s">
         <v>153</v>
       </c>
@@ -5376,7 +5376,7 @@
       <c r="F174" s="67"/>
       <c r="G174" s="67"/>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A175" s="55" t="s">
         <v>152</v>
       </c>
@@ -5389,7 +5389,7 @@
       <c r="F175" s="67"/>
       <c r="G175" s="67"/>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A176" s="55" t="s">
         <v>166</v>
       </c>
@@ -5402,7 +5402,7 @@
       <c r="F176" s="67"/>
       <c r="G176" s="67"/>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A177" s="55" t="s">
         <v>162</v>
       </c>
@@ -5415,7 +5415,7 @@
       <c r="F177" s="67"/>
       <c r="G177" s="67"/>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A178" s="55" t="s">
         <v>163</v>
       </c>
@@ -5428,7 +5428,7 @@
       <c r="F178" s="67"/>
       <c r="G178" s="67"/>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A179" s="55" t="s">
         <v>164</v>
       </c>
@@ -5441,7 +5441,7 @@
       <c r="F179" s="67"/>
       <c r="G179" s="67"/>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A180" s="55" t="s">
         <v>165</v>
       </c>
@@ -5454,7 +5454,7 @@
       <c r="F180" s="67"/>
       <c r="G180" s="67"/>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A181" s="55" t="s">
         <v>167</v>
       </c>
@@ -5467,7 +5467,7 @@
       <c r="F181" s="67"/>
       <c r="G181" s="67"/>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A182" s="55" t="s">
         <v>168</v>
       </c>
@@ -5480,7 +5480,7 @@
       <c r="F182" s="67"/>
       <c r="G182" s="67"/>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A183" s="55" t="s">
         <v>169</v>
       </c>
@@ -5493,7 +5493,7 @@
       <c r="F183" s="67"/>
       <c r="G183" s="67"/>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A184" s="55" t="s">
         <v>170</v>
       </c>
@@ -5506,7 +5506,7 @@
       <c r="F184" s="67"/>
       <c r="G184" s="67"/>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A185" s="55" t="s">
         <v>171</v>
       </c>
@@ -5519,7 +5519,7 @@
       <c r="F185" s="67"/>
       <c r="G185" s="67"/>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A186" s="55" t="s">
         <v>172</v>
       </c>
@@ -5532,7 +5532,7 @@
       <c r="F186" s="67"/>
       <c r="G186" s="67"/>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A187" s="55" t="s">
         <v>173</v>
       </c>
@@ -5545,7 +5545,7 @@
       <c r="F187" s="67"/>
       <c r="G187" s="67"/>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A188" s="55" t="s">
         <v>174</v>
       </c>
@@ -5558,7 +5558,7 @@
       <c r="F188" s="67"/>
       <c r="G188" s="67"/>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A189" s="55" t="s">
         <v>175</v>
       </c>
@@ -5571,7 +5571,7 @@
       <c r="F189" s="67"/>
       <c r="G189" s="67"/>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A190" s="55" t="s">
         <v>176</v>
       </c>
@@ -5584,7 +5584,7 @@
       <c r="F190" s="67"/>
       <c r="G190" s="67"/>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A191" s="55" t="s">
         <v>157</v>
       </c>
@@ -5597,7 +5597,7 @@
       <c r="F191" s="67"/>
       <c r="G191" s="67"/>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A192" s="55" t="s">
         <v>158</v>
       </c>
@@ -5610,7 +5610,7 @@
       <c r="F192" s="67"/>
       <c r="G192" s="67"/>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A193" s="55" t="s">
         <v>159</v>
       </c>
@@ -5621,7 +5621,7 @@
       <c r="D193" s="61"/>
       <c r="E193" s="55"/>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A194" s="55" t="s">
         <v>160</v>
       </c>
@@ -5632,7 +5632,7 @@
       <c r="D194" s="61"/>
       <c r="E194" s="74"/>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A195" s="55" t="s">
         <v>161</v>
       </c>
@@ -5643,7 +5643,7 @@
       <c r="D195" s="61"/>
       <c r="E195" s="74"/>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A196" s="55" t="s">
         <v>185</v>
       </c>
@@ -5654,7 +5654,7 @@
       <c r="D196" s="61"/>
       <c r="E196" s="74"/>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A197" s="55" t="s">
         <v>186</v>
       </c>
@@ -5665,7 +5665,7 @@
       <c r="D197" s="61"/>
       <c r="E197" s="74"/>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A198" s="55" t="s">
         <v>187</v>
       </c>
@@ -5676,7 +5676,7 @@
       <c r="D198" s="61"/>
       <c r="E198" s="74"/>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A199" s="55" t="s">
         <v>188</v>
       </c>
@@ -5687,7 +5687,7 @@
       <c r="D199" s="61"/>
       <c r="E199" s="74"/>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A200" s="55" t="s">
         <v>189</v>
       </c>
@@ -5698,7 +5698,7 @@
       <c r="D200" s="61"/>
       <c r="E200" s="74"/>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A201" s="55" t="s">
         <v>190</v>
       </c>
@@ -5709,7 +5709,7 @@
       <c r="D201" s="61"/>
       <c r="E201" s="74"/>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A202" s="55" t="s">
         <v>191</v>
       </c>
@@ -5720,7 +5720,7 @@
       <c r="D202" s="61"/>
       <c r="E202" s="74"/>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A203" s="55" t="s">
         <v>192</v>
       </c>
@@ -5731,7 +5731,7 @@
       <c r="D203" s="61"/>
       <c r="E203" s="74"/>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A204" s="55" t="s">
         <v>193</v>
       </c>
@@ -5742,7 +5742,7 @@
       <c r="D204" s="61"/>
       <c r="E204" s="74"/>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A205" s="55" t="s">
         <v>194</v>
       </c>
@@ -5753,7 +5753,7 @@
       <c r="D205" s="61"/>
       <c r="E205" s="74"/>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A206" s="55" t="s">
         <v>195</v>
       </c>
@@ -5764,7 +5764,7 @@
       <c r="D206" s="61"/>
       <c r="E206" s="74"/>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A207" s="55" t="s">
         <v>196</v>
       </c>
@@ -5775,7 +5775,7 @@
       <c r="D207" s="61"/>
       <c r="E207" s="74"/>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A208" s="55" t="s">
         <v>197</v>
       </c>
@@ -5786,7 +5786,7 @@
       <c r="D208" s="61"/>
       <c r="E208" s="74"/>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A209" s="55" t="s">
         <v>198</v>
       </c>
@@ -5797,7 +5797,7 @@
       <c r="D209" s="61"/>
       <c r="E209" s="74"/>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A210" s="55" t="s">
         <v>199</v>
       </c>
@@ -5808,7 +5808,7 @@
       <c r="D210" s="61"/>
       <c r="E210" s="74"/>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A211" s="55" t="s">
         <v>200</v>
       </c>
@@ -5819,7 +5819,7 @@
       <c r="D211" s="61"/>
       <c r="E211" s="74"/>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A212" s="55" t="s">
         <v>201</v>
       </c>
@@ -5830,7 +5830,7 @@
       <c r="D212" s="61"/>
       <c r="E212" s="74"/>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A213" s="55" t="s">
         <v>202</v>
       </c>
@@ -5841,7 +5841,7 @@
       <c r="D213" s="61"/>
       <c r="E213" s="74"/>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A214" s="55" t="s">
         <v>203</v>
       </c>
@@ -5852,7 +5852,7 @@
       <c r="D214" s="61"/>
       <c r="E214" s="74"/>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A215" s="55" t="s">
         <v>204</v>
       </c>
@@ -5863,7 +5863,7 @@
       <c r="D215" s="61"/>
       <c r="E215" s="74"/>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A216" s="55" t="s">
         <v>205</v>
       </c>
@@ -5874,7 +5874,7 @@
       <c r="D216" s="61"/>
       <c r="E216" s="74"/>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A217" s="55" t="s">
         <v>206</v>
       </c>
@@ -5885,7 +5885,7 @@
       <c r="D217" s="61"/>
       <c r="E217" s="74"/>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A218" s="55" t="s">
         <v>207</v>
       </c>
@@ -5896,7 +5896,7 @@
       <c r="D218" s="61"/>
       <c r="E218" s="74"/>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A219" s="55" t="s">
         <v>208</v>
       </c>
@@ -5907,7 +5907,7 @@
       <c r="D219" s="61"/>
       <c r="E219" s="55"/>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A220" s="55" t="s">
         <v>209</v>
       </c>
@@ -5918,7 +5918,7 @@
       <c r="D220" s="61"/>
       <c r="E220" s="55"/>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A221" s="55" t="s">
         <v>210</v>
       </c>
@@ -5929,7 +5929,7 @@
       <c r="D221" s="61"/>
       <c r="E221" s="55"/>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A222" s="55" t="s">
         <v>211</v>
       </c>
@@ -5940,7 +5940,7 @@
       <c r="D222" s="61"/>
       <c r="E222" s="55"/>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A223" s="55" t="s">
         <v>212</v>
       </c>
@@ -5951,7 +5951,7 @@
       <c r="D223" s="63"/>
       <c r="E223" s="52"/>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A224" s="55" t="s">
         <v>213</v>
       </c>
@@ -5962,7 +5962,7 @@
       <c r="D224" s="63"/>
       <c r="E224" s="52"/>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A225" s="55" t="s">
         <v>214</v>
       </c>
@@ -5973,7 +5973,7 @@
       <c r="D225" s="63"/>
       <c r="E225" s="52"/>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A226" s="55" t="s">
         <v>215</v>
       </c>
@@ -5984,7 +5984,7 @@
       <c r="D226" s="63"/>
       <c r="E226" s="52"/>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A227" s="55" t="s">
         <v>216</v>
       </c>
@@ -5995,7 +5995,7 @@
       <c r="D227" s="63"/>
       <c r="E227" s="52"/>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A228" s="55" t="s">
         <v>217</v>
       </c>
@@ -6006,7 +6006,7 @@
       <c r="D228" s="63"/>
       <c r="E228" s="52"/>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A229" s="55" t="s">
         <v>218</v>
       </c>
@@ -6017,7 +6017,7 @@
       <c r="D229" s="63"/>
       <c r="E229" s="52"/>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A230" s="55" t="s">
         <v>219</v>
       </c>
@@ -6028,7 +6028,7 @@
       <c r="D230" s="63"/>
       <c r="E230" s="52"/>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A231" s="55" t="s">
         <v>220</v>
       </c>
@@ -6039,7 +6039,7 @@
       <c r="D231" s="63"/>
       <c r="E231" s="52"/>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A232" s="55" t="s">
         <v>221</v>
       </c>
@@ -6050,7 +6050,7 @@
       <c r="D232" s="63"/>
       <c r="E232" s="52"/>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A233" s="55" t="s">
         <v>222</v>
       </c>
@@ -6061,7 +6061,7 @@
       <c r="D233" s="63"/>
       <c r="E233" s="52"/>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A234" s="55" t="s">
         <v>223</v>
       </c>
@@ -6072,7 +6072,7 @@
       <c r="D234" s="63"/>
       <c r="E234" s="52"/>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A235" s="55" t="s">
         <v>224</v>
       </c>
@@ -6083,7 +6083,7 @@
       <c r="D235" s="63"/>
       <c r="E235" s="52"/>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A236" s="55" t="s">
         <v>231</v>
       </c>
@@ -6096,7 +6096,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A237" s="55" t="s">
         <v>232</v>
       </c>
@@ -6109,7 +6109,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A238" s="55" t="s">
         <v>233</v>
       </c>
@@ -6122,7 +6122,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A239" s="55" t="s">
         <v>234</v>
       </c>
@@ -6135,7 +6135,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A240" s="55" t="s">
         <v>235</v>
       </c>
@@ -6148,7 +6148,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A241" s="55" t="s">
         <v>237</v>
       </c>
@@ -6162,7 +6162,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A242" s="55" t="s">
         <v>238</v>
       </c>
@@ -6175,7 +6175,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A243" s="55" t="s">
         <v>239</v>
       </c>
@@ -6188,7 +6188,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A244" s="55" t="s">
         <v>240</v>
       </c>
@@ -6201,7 +6201,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A245" s="55" t="s">
         <v>241</v>
       </c>
@@ -6214,7 +6214,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A246" s="55" t="s">
         <v>242</v>
       </c>
@@ -6228,7 +6228,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A247" s="55" t="s">
         <v>243</v>
       </c>
@@ -6241,7 +6241,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A248" s="55" t="s">
         <v>244</v>
       </c>
@@ -6254,7 +6254,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A249" s="55" t="s">
         <v>245</v>
       </c>
@@ -6267,7 +6267,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A250" s="55" t="s">
         <v>246</v>
       </c>
@@ -6280,7 +6280,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A251" s="55" t="s">
         <v>247</v>
       </c>
@@ -6291,7 +6291,7 @@
       <c r="D251" s="63"/>
       <c r="E251" s="52"/>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A252" s="55" t="s">
         <v>248</v>
       </c>
@@ -6302,7 +6302,7 @@
       <c r="D252" s="63"/>
       <c r="E252" s="52"/>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A253" s="55" t="s">
         <v>249</v>
       </c>
@@ -6313,7 +6313,7 @@
       <c r="D253" s="63"/>
       <c r="E253" s="52"/>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A254" s="55" t="s">
         <v>250</v>
       </c>
@@ -6324,7 +6324,7 @@
       <c r="D254" s="63"/>
       <c r="E254" s="52"/>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A255" s="55" t="s">
         <v>251</v>
       </c>
@@ -6335,7 +6335,7 @@
       <c r="D255" s="63"/>
       <c r="E255" s="52"/>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A256" s="78" t="s">
         <v>280</v>
       </c>
@@ -6346,7 +6346,7 @@
       <c r="D256" s="79"/>
       <c r="E256" s="77"/>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A257" s="78" t="s">
         <v>281</v>
       </c>
@@ -6357,7 +6357,7 @@
       <c r="D257" s="79"/>
       <c r="E257" s="77"/>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A258" s="78" t="s">
         <v>282</v>
       </c>
@@ -6368,7 +6368,7 @@
       <c r="D258" s="79"/>
       <c r="E258" s="77"/>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A259" s="78" t="s">
         <v>283</v>
       </c>
@@ -6379,7 +6379,7 @@
       <c r="D259" s="79"/>
       <c r="E259" s="77"/>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A260" s="78" t="s">
         <v>284</v>
       </c>
@@ -6390,7 +6390,7 @@
       <c r="D260" s="79"/>
       <c r="E260" s="77"/>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A261" s="78" t="s">
         <v>285</v>
       </c>
@@ -6401,7 +6401,7 @@
       <c r="D261" s="79"/>
       <c r="E261" s="77"/>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A262" s="78" t="s">
         <v>286</v>
       </c>
@@ -6412,7 +6412,7 @@
       <c r="D262" s="79"/>
       <c r="E262" s="77"/>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A263" s="78" t="s">
         <v>287</v>
       </c>
@@ -6423,7 +6423,7 @@
       <c r="D263" s="79"/>
       <c r="E263" s="77"/>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A264" s="78" t="s">
         <v>288</v>
       </c>
@@ -6434,7 +6434,7 @@
       <c r="D264" s="79"/>
       <c r="E264" s="77"/>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A265" s="87" t="s">
         <v>289</v>
       </c>
@@ -6445,7 +6445,7 @@
       <c r="D265" s="88"/>
       <c r="E265" s="87"/>
     </row>
-    <row r="266" spans="1:5" s="86" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:5" s="86" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A266" s="78" t="s">
         <v>351</v>
       </c>
@@ -6458,7 +6458,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="267" spans="1:5" s="86" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:5" s="86" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A267" s="78" t="s">
         <v>352</v>
       </c>
@@ -6471,7 +6471,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="268" spans="1:5" s="86" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:5" s="86" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A268" s="78" t="s">
         <v>353</v>
       </c>
@@ -6484,7 +6484,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="269" spans="1:5" s="86" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:5" s="86" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A269" s="78" t="s">
         <v>354</v>
       </c>
@@ -6497,7 +6497,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A270" s="78" t="s">
         <v>355</v>
       </c>
@@ -6510,7 +6510,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="271" spans="1:5" s="91" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:5" s="91" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A271" s="91" t="s">
         <v>366</v>
       </c>
@@ -6521,7 +6521,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="272" spans="1:5" s="91" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:5" s="91" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A272" s="91" t="s">
         <v>368</v>
       </c>
@@ -6529,7 +6529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="273" spans="1:5" s="91" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:5" s="91" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A273" s="91" t="s">
         <v>369</v>
       </c>
@@ -6537,7 +6537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="274" spans="1:5" s="91" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:5" s="91" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A274" s="91" t="s">
         <v>370</v>
       </c>
@@ -6545,7 +6545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="275" spans="1:5" s="91" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:5" s="91" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A275" s="91" t="s">
         <v>371</v>
       </c>
@@ -6553,7 +6553,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="276" spans="1:5" s="91" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:5" s="91" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A276" s="91" t="s">
         <v>372</v>
       </c>
@@ -6564,7 +6564,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="277" spans="1:5" s="91" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:5" s="91" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A277" s="91" t="s">
         <v>373</v>
       </c>
@@ -6572,7 +6572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="278" spans="1:5" s="91" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:5" s="91" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A278" s="91" t="s">
         <v>374</v>
       </c>
@@ -6580,7 +6580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="279" spans="1:5" s="91" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:5" s="91" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A279" s="91" t="s">
         <v>375</v>
       </c>
@@ -6588,7 +6588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="280" spans="1:5" s="91" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:5" s="91" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A280" s="91" t="s">
         <v>376</v>
       </c>
@@ -6623,30 +6623,30 @@
   <dimension ref="A1:M39"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H33" sqref="H33"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="61.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="61.54296875" style="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" style="2" customWidth="1"/>
-    <col min="4" max="4" width="7.42578125" style="1" customWidth="1"/>
-    <col min="5" max="6" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="7.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="7.42578125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.85546875" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="7.453125" style="1" customWidth="1"/>
+    <col min="5" max="6" width="7.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.453125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="7.26953125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="7.453125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="10.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.81640625" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -6687,7 +6687,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="41" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" s="41" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="39" t="s">
         <v>267</v>
       </c>
@@ -6708,7 +6708,7 @@
       <c r="L2" s="45"/>
       <c r="M2" s="45"/>
     </row>
-    <row r="3" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>332</v>
       </c>
@@ -6731,7 +6731,7 @@
       </c>
       <c r="M3" s="48"/>
     </row>
-    <row r="4" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
         <v>333</v>
       </c>
@@ -6752,7 +6752,7 @@
       </c>
       <c r="M4" s="48"/>
     </row>
-    <row r="5" spans="1:13" s="21" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="19" t="s">
         <v>91</v>
       </c>
@@ -6773,7 +6773,7 @@
       <c r="L5" s="46"/>
       <c r="M5" s="46"/>
     </row>
-    <row r="6" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="14" t="s">
         <v>92</v>
       </c>
@@ -6794,7 +6794,7 @@
       <c r="L6" s="47"/>
       <c r="M6" s="47"/>
     </row>
-    <row r="7" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="14" t="s">
         <v>357</v>
       </c>
@@ -6819,7 +6819,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="14" t="s">
         <v>358</v>
       </c>
@@ -6842,7 +6842,7 @@
       <c r="L8" s="47"/>
       <c r="M8" s="47"/>
     </row>
-    <row r="9" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="16" t="s">
         <v>304</v>
       </c>
@@ -6863,7 +6863,7 @@
       <c r="L9" s="49"/>
       <c r="M9" s="49"/>
     </row>
-    <row r="10" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="16" t="s">
         <v>337</v>
       </c>
@@ -6884,7 +6884,7 @@
       <c r="L10" s="49"/>
       <c r="M10" s="49"/>
     </row>
-    <row r="11" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="16" t="s">
         <v>305</v>
       </c>
@@ -6907,7 +6907,7 @@
       <c r="L11" s="49"/>
       <c r="M11" s="49"/>
     </row>
-    <row r="12" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="16" t="s">
         <v>338</v>
       </c>
@@ -6930,7 +6930,7 @@
       <c r="L12" s="49"/>
       <c r="M12" s="49"/>
     </row>
-    <row r="13" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="16" t="s">
         <v>306</v>
       </c>
@@ -6955,7 +6955,7 @@
       <c r="L13" s="49"/>
       <c r="M13" s="49"/>
     </row>
-    <row r="14" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="16" t="s">
         <v>339</v>
       </c>
@@ -6978,7 +6978,7 @@
       <c r="L14" s="49"/>
       <c r="M14" s="49"/>
     </row>
-    <row r="15" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="16" t="s">
         <v>291</v>
       </c>
@@ -6999,7 +6999,7 @@
       <c r="L15" s="49"/>
       <c r="M15" s="49"/>
     </row>
-    <row r="16" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="16" t="s">
         <v>340</v>
       </c>
@@ -7020,7 +7020,7 @@
       <c r="L16" s="49"/>
       <c r="M16" s="49"/>
     </row>
-    <row r="17" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="16" t="s">
         <v>292</v>
       </c>
@@ -7041,7 +7041,7 @@
       <c r="L17" s="49"/>
       <c r="M17" s="49"/>
     </row>
-    <row r="18" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="16" t="s">
         <v>341</v>
       </c>
@@ -7062,7 +7062,7 @@
       <c r="L18" s="49"/>
       <c r="M18" s="49"/>
     </row>
-    <row r="19" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="16" t="s">
         <v>293</v>
       </c>
@@ -7083,7 +7083,7 @@
       <c r="L19" s="49"/>
       <c r="M19" s="49"/>
     </row>
-    <row r="20" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="16" t="s">
         <v>342</v>
       </c>
@@ -7104,7 +7104,7 @@
       <c r="L20" s="49"/>
       <c r="M20" s="49"/>
     </row>
-    <row r="21" spans="1:13" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" s="44" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="42" t="s">
         <v>294</v>
       </c>
@@ -7129,7 +7129,7 @@
       <c r="L21" s="50"/>
       <c r="M21" s="50"/>
     </row>
-    <row r="22" spans="1:13" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" s="44" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="42" t="s">
         <v>343</v>
       </c>
@@ -7152,7 +7152,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="23" spans="1:13" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" s="44" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="42" t="s">
         <v>295</v>
       </c>
@@ -7175,7 +7175,7 @@
       <c r="L23" s="50"/>
       <c r="M23" s="50"/>
     </row>
-    <row r="24" spans="1:13" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" s="44" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="42" t="s">
         <v>344</v>
       </c>
@@ -7196,7 +7196,7 @@
       <c r="L24" s="50"/>
       <c r="M24" s="50"/>
     </row>
-    <row r="25" spans="1:13" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" s="44" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="42" t="s">
         <v>296</v>
       </c>
@@ -7219,7 +7219,7 @@
       <c r="L25" s="50"/>
       <c r="M25" s="50"/>
     </row>
-    <row r="26" spans="1:13" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" s="44" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="42" t="s">
         <v>345</v>
       </c>
@@ -7240,7 +7240,7 @@
       <c r="L26" s="50"/>
       <c r="M26" s="50"/>
     </row>
-    <row r="27" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="17" t="s">
         <v>297</v>
       </c>
@@ -7265,7 +7265,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="17" t="s">
         <v>346</v>
       </c>
@@ -7288,7 +7288,7 @@
       <c r="L28" s="51"/>
       <c r="M28" s="51"/>
     </row>
-    <row r="29" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="17" t="s">
         <v>298</v>
       </c>
@@ -7313,7 +7313,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="17" t="s">
         <v>347</v>
       </c>
@@ -7336,7 +7336,7 @@
       <c r="L30" s="51"/>
       <c r="M30" s="51"/>
     </row>
-    <row r="31" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="17" t="s">
         <v>299</v>
       </c>
@@ -7361,7 +7361,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="17" t="s">
         <v>347</v>
       </c>
@@ -7384,7 +7384,7 @@
       <c r="L32" s="51"/>
       <c r="M32" s="51"/>
     </row>
-    <row r="33" spans="1:13" s="83" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" s="83" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="80" t="s">
         <v>300</v>
       </c>
@@ -7407,7 +7407,7 @@
       <c r="L33" s="82"/>
       <c r="M33" s="82"/>
     </row>
-    <row r="34" spans="1:13" s="83" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" s="83" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="80" t="s">
         <v>348</v>
       </c>
@@ -7430,7 +7430,7 @@
       <c r="L34" s="82"/>
       <c r="M34" s="82"/>
     </row>
-    <row r="35" spans="1:13" s="83" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" s="83" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="80" t="s">
         <v>301</v>
       </c>
@@ -7453,7 +7453,7 @@
       <c r="L35" s="82"/>
       <c r="M35" s="82"/>
     </row>
-    <row r="36" spans="1:13" s="83" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" s="83" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A36" s="80" t="s">
         <v>349</v>
       </c>
@@ -7476,7 +7476,7 @@
       <c r="L36" s="82"/>
       <c r="M36" s="82"/>
     </row>
-    <row r="37" spans="1:13" s="83" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" s="83" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A37" s="80" t="s">
         <v>302</v>
       </c>
@@ -7499,7 +7499,7 @@
       <c r="L37" s="82"/>
       <c r="M37" s="82"/>
     </row>
-    <row r="38" spans="1:13" s="83" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" s="83" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A38" s="80" t="s">
         <v>350</v>
       </c>
@@ -7522,7 +7522,7 @@
       <c r="L38" s="82"/>
       <c r="M38" s="82"/>
     </row>
-    <row r="39" spans="1:13" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" s="44" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A39" s="42" t="s">
         <v>66</v>
       </c>
@@ -7595,9 +7595,9 @@
       <selection activeCell="D4" sqref="A2:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -7611,7 +7611,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -7622,7 +7622,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>

</xml_diff>